<commit_message>
Fix WP43 layout in C43
</commit_message>
<xml_diff>
--- a/src/index spreadsheet/WP43S key template.xlsx
+++ b/src/index spreadsheet/WP43S key template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacomostert/wp43s/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacomostert/wp43s/src/index spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92933DE-5B6D-E14D-926C-1FD84ABA8B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E30A00D-E60F-EE44-8DD5-C80E6D53FD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27300" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="import" sheetId="1" r:id="rId1"/>
-    <sheet name="output code" sheetId="2" r:id="rId2"/>
+    <sheet name="Latest import 2022-10-10" sheetId="3" r:id="rId2"/>
+    <sheet name="output code" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="305">
   <si>
     <t>primary</t>
   </si>
@@ -750,6 +751,204 @@
   </si>
   <si>
     <t>ITM_UP1</t>
+  </si>
+  <si>
+    <t>{21</t>
+  </si>
+  <si>
+    <t>{22</t>
+  </si>
+  <si>
+    <t>{23</t>
+  </si>
+  <si>
+    <t>{24</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
+    <t>changed:</t>
+  </si>
+  <si>
+    <t>adapt</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>btnClicked</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>if(calcMode</t>
+  </si>
+  <si>
+    <t>==</t>
+  </si>
+  <si>
+    <t>cmNim)</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>keyboard.c.</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>{25</t>
+  </si>
+  <si>
+    <t>{26</t>
+  </si>
+  <si>
+    <t>{31</t>
+  </si>
+  <si>
+    <t>{32</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>hexadecimal</t>
+  </si>
+  <si>
+    <t>{33</t>
+  </si>
+  <si>
+    <t>{34</t>
+  </si>
+  <si>
+    <t>{35</t>
+  </si>
+  <si>
+    <t>{36</t>
+  </si>
+  <si>
+    <t>{41</t>
+  </si>
+  <si>
+    <t>{42</t>
+  </si>
+  <si>
+    <t>{43</t>
+  </si>
+  <si>
+    <t>{44</t>
+  </si>
+  <si>
+    <t>{45</t>
+  </si>
+  <si>
+    <t>{51</t>
+  </si>
+  <si>
+    <t>ITM_PARALLEL</t>
+  </si>
+  <si>
+    <t>{52</t>
+  </si>
+  <si>
+    <t>{53</t>
+  </si>
+  <si>
+    <t>{54</t>
+  </si>
+  <si>
+    <t>ITM_OMICRON</t>
+  </si>
+  <si>
+    <t>{55</t>
+  </si>
+  <si>
+    <t>{61</t>
+  </si>
+  <si>
+    <t>{62</t>
+  </si>
+  <si>
+    <t>{63</t>
+  </si>
+  <si>
+    <t>{64</t>
+  </si>
+  <si>
+    <t>{65</t>
+  </si>
+  <si>
+    <t>ITM_UP</t>
+  </si>
+  <si>
+    <t>{71</t>
+  </si>
+  <si>
+    <t>{72</t>
+  </si>
+  <si>
+    <t>{73</t>
+  </si>
+  <si>
+    <t>{74</t>
+  </si>
+  <si>
+    <t>{75</t>
+  </si>
+  <si>
+    <t>ITM_DOWN</t>
+  </si>
+  <si>
+    <t>{81</t>
+  </si>
+  <si>
+    <t>{82</t>
+  </si>
+  <si>
+    <t>{83</t>
+  </si>
+  <si>
+    <t>{84</t>
+  </si>
+  <si>
+    <t>{85</t>
+  </si>
+  <si>
+    <t>ITM_EXIT</t>
   </si>
 </sst>
 </file>
@@ -788,36 +987,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -864,17 +1039,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -911,7 +1083,228 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1249,1233 +1642,1307 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="3" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="3" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="3" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I25" t="s">
-        <v>144</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="F26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" t="s">
-        <v>110</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" t="s">
-        <v>110</v>
-      </c>
-      <c r="I26" t="s">
-        <v>10</v>
-      </c>
-      <c r="J26" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" t="s">
-        <v>201</v>
-      </c>
-      <c r="F28" t="s">
-        <v>202</v>
-      </c>
-      <c r="G28" t="s">
-        <v>203</v>
-      </c>
-      <c r="H28" t="s">
-        <v>204</v>
-      </c>
-      <c r="I28" t="s">
-        <v>45</v>
-      </c>
-      <c r="J28" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J29" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" t="s">
-        <v>145</v>
-      </c>
-      <c r="F29" t="s">
-        <v>205</v>
-      </c>
-      <c r="G29" t="s">
-        <v>145</v>
-      </c>
-      <c r="H29" t="s">
-        <v>206</v>
-      </c>
-      <c r="I29" t="s">
-        <v>145</v>
-      </c>
-      <c r="J29" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" t="s">
-        <v>146</v>
-      </c>
-      <c r="C30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" t="s">
-        <v>146</v>
-      </c>
-      <c r="F30" t="s">
-        <v>207</v>
-      </c>
-      <c r="G30" t="s">
-        <v>146</v>
-      </c>
-      <c r="H30" t="s">
-        <v>208</v>
-      </c>
-      <c r="I30" t="s">
-        <v>146</v>
-      </c>
-      <c r="J30" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J31" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" t="s">
-        <v>147</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" t="s">
-        <v>147</v>
-      </c>
-      <c r="F31" t="s">
-        <v>209</v>
-      </c>
-      <c r="G31" t="s">
-        <v>147</v>
-      </c>
-      <c r="H31" t="s">
-        <v>210</v>
-      </c>
-      <c r="I31" t="s">
-        <v>147</v>
-      </c>
-      <c r="J31" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="J32" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C32" t="s">
-        <v>211</v>
-      </c>
-      <c r="D32" t="s">
-        <v>234</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G32" t="s">
-        <v>211</v>
-      </c>
-      <c r="H32" t="s">
-        <v>234</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="J32" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J34" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J34" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J35" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="J35" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="J36" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="J36" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J37" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="J37" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="J38" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="J38" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J40" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" t="s">
-        <v>123</v>
-      </c>
-      <c r="E40" t="s">
-        <v>222</v>
-      </c>
-      <c r="F40" t="s">
-        <v>223</v>
-      </c>
-      <c r="G40" t="s">
-        <v>222</v>
-      </c>
-      <c r="H40" t="s">
-        <v>224</v>
-      </c>
-      <c r="I40" t="s">
-        <v>51</v>
-      </c>
-      <c r="J40" t="s">
-        <v>56</v>
-      </c>
-    </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="3" t="s">
         <v>151</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2483,6 +2950,26 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{2C0972BE-567C-5A45-A383-606A03975E40}">
+            <xm:f>FIND('Latest import 2022-10-10'!A1,A1)</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A1:I44</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
@@ -2491,6 +2978,1367 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F600D62E-3D15-1E40-B755-B91BDA236CA7}">
+  <dimension ref="A2:AF44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L5" t="s">
+        <v>244</v>
+      </c>
+      <c r="M5" t="s">
+        <v>245</v>
+      </c>
+      <c r="N5" t="s">
+        <v>246</v>
+      </c>
+      <c r="O5" t="s">
+        <v>247</v>
+      </c>
+      <c r="P5" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>249</v>
+      </c>
+      <c r="R5" t="s">
+        <v>250</v>
+      </c>
+      <c r="S5" t="s">
+        <v>251</v>
+      </c>
+      <c r="T5" t="s">
+        <v>252</v>
+      </c>
+      <c r="U5" t="s">
+        <v>253</v>
+      </c>
+      <c r="V5" t="s">
+        <v>254</v>
+      </c>
+      <c r="W5" t="s">
+        <v>255</v>
+      </c>
+      <c r="X5" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>258</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>259</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>263</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="L10" t="s">
+        <v>244</v>
+      </c>
+      <c r="M10" t="s">
+        <v>245</v>
+      </c>
+      <c r="N10" t="s">
+        <v>246</v>
+      </c>
+      <c r="O10" t="s">
+        <v>247</v>
+      </c>
+      <c r="P10" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>249</v>
+      </c>
+      <c r="R10" t="s">
+        <v>250</v>
+      </c>
+      <c r="S10" t="s">
+        <v>251</v>
+      </c>
+      <c r="T10" t="s">
+        <v>252</v>
+      </c>
+      <c r="U10" t="s">
+        <v>253</v>
+      </c>
+      <c r="V10" t="s">
+        <v>254</v>
+      </c>
+      <c r="W10" t="s">
+        <v>255</v>
+      </c>
+      <c r="X10" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>258</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>259</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>260</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>269</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>270</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
@@ -3315,7 +5163,7 @@
       </c>
       <c r="H22" t="str">
         <f>"kbd_usr["&amp;$A22&amp;"]."&amp;H$1&amp;"="&amp;import!H25&amp;"; "</f>
-        <v xml:space="preserve">kbd_usr[20].gShiftedAim=ITM_NULL; </v>
+        <v xml:space="preserve">kbd_usr[20].gShiftedAim=ITM_OMICRON; </v>
       </c>
       <c r="I22" t="str">
         <f>"kbd_usr["&amp;$A22&amp;"]."&amp;I$1&amp;"="&amp;import!I25&amp;"; "</f>

</xml_diff>